<commit_message>
fixing semaine and emploi excel
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/ImporterClasse.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/ImporterClasse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Nom</t>
   </si>
@@ -32,12 +32,27 @@
     <t>Cycle</t>
   </si>
   <si>
+    <t>Cp 2</t>
+  </si>
+  <si>
     <t>CP</t>
   </si>
   <si>
     <t>CI</t>
   </si>
   <si>
+    <t>4.GTR</t>
+  </si>
+  <si>
+    <t>Cp 1</t>
+  </si>
+  <si>
+    <t>3.GTR</t>
+  </si>
+  <si>
+    <t>5.GTR</t>
+  </si>
+  <si>
     <t>3.GPMC</t>
   </si>
   <si>
@@ -47,22 +62,22 @@
     <t>5.GPMC</t>
   </si>
   <si>
-    <t>3.GTR</t>
-  </si>
-  <si>
-    <t>5.GTR</t>
-  </si>
-  <si>
     <t>3.INDUS</t>
   </si>
   <si>
+    <t>3.GINFO</t>
+  </si>
+  <si>
+    <t>4.GINFO</t>
+  </si>
+  <si>
+    <t>5.GINFO</t>
+  </si>
+  <si>
     <t>4.INDUS</t>
   </si>
   <si>
     <t>5.INDUS</t>
-  </si>
-  <si>
-    <t>Cp 1</t>
   </si>
 </sst>
 </file>
@@ -380,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F5:G14"/>
+  <dimension ref="F5:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,31 +413,31 @@
     </row>
     <row r="6" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
         <v>3</v>
@@ -430,7 +445,7 @@
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -438,34 +453,74 @@
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>12</v>
       </c>
-      <c r="G14" t="s">
-        <v>2</v>
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>